<commit_message>
100% Funcionalidad y Estilos - falta Responsividad
</commit_message>
<xml_diff>
--- a/Libro_db.xlsx
+++ b/Libro_db.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>0539021b-d4aa-4540-8775-6b192efedaa8</t>
   </si>
@@ -69,9 +69,6 @@
     <t>paleolithic</t>
   </si>
   <si>
-    <t>{Invitar,llevar,pedir,brindar,"observar su rostro de satisfaccion"}</t>
-  </si>
-  <si>
     <t>Mandocas</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>{"Busca un pan campesino","rellenar con vegetales de su preferencia","agregar jamon, queso, salami y peperoni","Condimentar con salsas de su preferencia","Agregar encurtidos varios como jalapenos, aceitunasnegras, palmito, maiz y champinon'"}</t>
   </si>
   <si>
-    <t>https://c.wallhere.com/photos/de/ca/food_sandwiches-216633.jpg!d</t>
-  </si>
-  <si>
     <t>{"Preparar Base de Salsa Carbonara","Trocear y hornear 500Gr de Tocineta","Preprar la Pata al Gusto","Mezclar y agregar queso parmesano o pecorino al gusto"}</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>Pizza de masa esponjosa con hongos, queso Roquefort y especias mediterraneas</t>
+  </si>
+  <si>
+    <t>{"Comprar 50 gr de masa para pizza lista","extender en molde enmantecado","cubrir con salsa para pizza al gusto","agregar 150 gr de queso mozzarella","incorporar 50 gr de queso Roquefort","agregar los ongos y las especia al gusto","hornear a 180 por 15 min"}</t>
+  </si>
+  <si>
+    <t>https://c.wallhere.com/photos/de/ca/food_sandwiches-216633.jpg</t>
   </si>
 </sst>
 </file>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,25 +586,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -612,22 +612,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="F2" s="4">
         <v>100</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -635,45 +635,45 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="4">
         <v>85</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="4">
         <v>78</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -681,22 +681,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4">
         <v>80</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -704,22 +704,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="4">
         <v>75</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -727,22 +727,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="4">
         <v>100</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -750,47 +750,81 @@
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="4">
         <v>68</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="4">
         <v>72</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -809,7 +843,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -817,7 +851,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -825,7 +859,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -833,7 +867,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -841,7 +875,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -849,7 +883,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -865,32 +899,32 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>